<commit_message>
task.feature ac-5 added and location of test data change
</commit_message>
<xml_diff>
--- a/SaveYourData.xlsx
+++ b/SaveYourData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CNON\IdeaProjects\G22_LastAgileProCRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A7BD95-EA01-4160-BEA6-DB1118BF10F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE42F4F-1430-4D51-A51F-132A23FD325D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="16416" windowHeight="28416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WriteYourName" sheetId="2" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">IF YOU WANT TO USE EXCEL SHEET, PLEASE CREATE NEW SHEET WITH YOUR BRANCH NAME </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="9">
   <si>
     <t>Null</t>
   </si>
@@ -43,28 +40,19 @@
     <t>User Story/Variable Definition</t>
   </si>
   <si>
-    <t>Task -255</t>
+    <t>Task -411</t>
   </si>
   <si>
-    <t>Task -360</t>
+    <t xml:space="preserve">IF YOU WANT TO USE EXCEL SHEET, PLEASE CREATE A NEW SHEET WITH YOUR BRANCH NAME </t>
   </si>
   <si>
-    <t>Task -869</t>
+    <t>Task -122</t>
   </si>
   <si>
-    <t>Task -300</t>
+    <t>Task -502</t>
   </si>
   <si>
-    <t>Task -002</t>
-  </si>
-  <si>
-    <t>Task -882</t>
-  </si>
-  <si>
-    <t>Task -786</t>
-  </si>
-  <si>
-    <t>Task -755</t>
+    <t>Task -834</t>
   </si>
 </sst>
 </file>
@@ -128,9 +116,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -139,6 +124,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,123 +410,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD60061-744A-4584-9D8E-0F045E974A59}">
   <dimension ref="A4:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -553,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -564,226 +552,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>1</v>
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>1</v>
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>1</v>
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>1</v>
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>1</v>
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>1</v>
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>1</v>
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>

</xml_diff>

<commit_message>
new test suite moneyTrans created
</commit_message>
<xml_diff>
--- a/SaveYourData.xlsx
+++ b/SaveYourData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
   <si>
     <t>Null</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Task -249</t>
+  </si>
+  <si>
+    <t>Task -128</t>
+  </si>
+  <si>
+    <t>Task -897</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>

</xml_diff>